<commit_message>
basics of queue | implementation of Queue
</commit_message>
<xml_diff>
--- a/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nimit\Downloads\other\study\java-practice-programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECD97F1-F836-4986-B925-032E955311D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B628722D-97BB-4C69-AEDC-FF2CF13FEED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{C68DABDE-8AC1-49C3-98CF-691EE57ABE88}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{FB58D069-98FB-40A6-98B6-6F873CC8E3CF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{A6CE0597-98E5-4A5B-AB5F-6EEE71119C0A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{DB562CAF-E1A0-40F3-9192-5E17BE155BA5}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{A6CE0597-98E5-4A5B-AB5F-6EEE71119C0A}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{FB58D069-98FB-40A6-98B6-6F873CC8E3CF}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{C68DABDE-8AC1-49C3-98CF-691EE57ABE88}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -2350,7 +2350,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2435,6 +2435,12 @@
         <bgColor rgb="FFA2C4C9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2448,7 +2454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2571,16 +2577,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2606,6 +2602,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2827,8 +2836,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153:XFD153"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2841,12 +2850,12 @@
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2869,12 +2878,12 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2896,10 +2905,10 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2924,10 +2933,10 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="60"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2950,7 +2959,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2978,7 +2987,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3008,14 +3017,14 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="62" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2"/>
@@ -3040,14 +3049,14 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="49"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -3070,7 +3079,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="7"/>
@@ -3096,7 +3105,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3122,7 +3131,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
@@ -3156,7 +3165,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -3188,7 +3197,7 @@
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
     </row>
-    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -3220,7 +3229,7 @@
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
@@ -3254,7 +3263,7 @@
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
     </row>
-    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -3286,7 +3295,7 @@
       <c r="W15" s="2"/>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -3318,7 +3327,7 @@
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
     </row>
-    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -3350,7 +3359,7 @@
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
     </row>
-    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
@@ -3382,7 +3391,7 @@
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
     </row>
-    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
         <v>14</v>
       </c>
@@ -3414,7 +3423,7 @@
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
     </row>
-    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
@@ -3446,7 +3455,7 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
     </row>
-    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="8" t="s">
         <v>14</v>
       </c>
@@ -3478,7 +3487,7 @@
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
     </row>
-    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="8" t="s">
         <v>14</v>
       </c>
@@ -3510,7 +3519,7 @@
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
     </row>
-    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="8" t="s">
         <v>14</v>
       </c>
@@ -3542,7 +3551,7 @@
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
     </row>
-    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
         <v>14</v>
       </c>
@@ -3574,7 +3583,7 @@
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="8" t="s">
         <v>14</v>
       </c>
@@ -3606,7 +3615,7 @@
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="8" t="s">
         <v>14</v>
       </c>
@@ -3638,7 +3647,7 @@
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
     </row>
-    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
@@ -3670,7 +3679,7 @@
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
     </row>
-    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="8" t="s">
         <v>14</v>
       </c>
@@ -3702,7 +3711,7 @@
       <c r="W28" s="2"/>
       <c r="X28" s="2"/>
     </row>
-    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
         <v>14</v>
       </c>
@@ -3734,7 +3743,7 @@
       <c r="W29" s="2"/>
       <c r="X29" s="2"/>
     </row>
-    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="8" t="s">
         <v>14</v>
       </c>
@@ -3766,7 +3775,7 @@
       <c r="W30" s="2"/>
       <c r="X30" s="2"/>
     </row>
-    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="8" t="s">
         <v>14</v>
       </c>
@@ -3798,7 +3807,7 @@
       <c r="W31" s="2"/>
       <c r="X31" s="2"/>
     </row>
-    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="8" t="s">
         <v>14</v>
       </c>
@@ -3830,7 +3839,7 @@
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
     </row>
-    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="8" t="s">
         <v>14</v>
       </c>
@@ -3862,7 +3871,7 @@
       <c r="W33" s="2"/>
       <c r="X33" s="2"/>
     </row>
-    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="8" t="s">
         <v>14</v>
       </c>
@@ -3894,7 +3903,7 @@
       <c r="W34" s="2"/>
       <c r="X34" s="2"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
         <v>14</v>
       </c>
@@ -3926,7 +3935,7 @@
       <c r="W35" s="2"/>
       <c r="X35" s="2"/>
     </row>
-    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="9" t="s">
         <v>14</v>
       </c>
@@ -3958,7 +3967,7 @@
       <c r="W36" s="2"/>
       <c r="X36" s="2"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="9" t="s">
         <v>14</v>
       </c>
@@ -3990,7 +3999,7 @@
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
     </row>
-    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="16"/>
       <c r="B38" s="17"/>
       <c r="C38" s="7"/>
@@ -4016,7 +4025,7 @@
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
     </row>
-    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="16"/>
       <c r="B39" s="17"/>
       <c r="C39" s="7"/>
@@ -4042,7 +4051,7 @@
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
     </row>
-    <row r="40" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="43" t="s">
         <v>61</v>
       </c>
@@ -4074,7 +4083,7 @@
       <c r="W40" s="46"/>
       <c r="X40" s="46"/>
     </row>
-    <row r="41" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="43" t="s">
         <v>61</v>
       </c>
@@ -4106,7 +4115,7 @@
       <c r="W41" s="46"/>
       <c r="X41" s="46"/>
     </row>
-    <row r="42" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="43" t="s">
         <v>61</v>
       </c>
@@ -4140,7 +4149,7 @@
       <c r="W42" s="46"/>
       <c r="X42" s="46"/>
     </row>
-    <row r="43" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="43" t="s">
         <v>61</v>
       </c>
@@ -4172,7 +4181,7 @@
       <c r="W43" s="46"/>
       <c r="X43" s="46"/>
     </row>
-    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5" t="s">
         <v>61</v>
       </c>
@@ -4204,7 +4213,7 @@
       <c r="W44" s="2"/>
       <c r="X44" s="2"/>
     </row>
-    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>61</v>
       </c>
@@ -4236,7 +4245,7 @@
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
     </row>
-    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
         <v>61</v>
       </c>
@@ -4268,7 +4277,7 @@
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
     </row>
-    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="8" t="s">
         <v>61</v>
       </c>
@@ -4300,7 +4309,7 @@
       <c r="W47" s="2"/>
       <c r="X47" s="2"/>
     </row>
-    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="8" t="s">
         <v>61</v>
       </c>
@@ -4332,7 +4341,7 @@
       <c r="W48" s="2"/>
       <c r="X48" s="2"/>
     </row>
-    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="8" t="s">
         <v>61</v>
       </c>
@@ -4364,7 +4373,7 @@
       <c r="W49" s="2"/>
       <c r="X49" s="2"/>
     </row>
-    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="8" t="s">
         <v>61</v>
       </c>
@@ -4396,7 +4405,7 @@
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
     </row>
-    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="8" t="s">
         <v>61</v>
       </c>
@@ -4428,7 +4437,7 @@
       <c r="W51" s="2"/>
       <c r="X51" s="2"/>
     </row>
-    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="8" t="s">
         <v>61</v>
       </c>
@@ -4460,7 +4469,7 @@
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
     </row>
-    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="8" t="s">
         <v>61</v>
       </c>
@@ -4492,7 +4501,7 @@
       <c r="W53" s="2"/>
       <c r="X53" s="2"/>
     </row>
-    <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="8" t="s">
         <v>61</v>
       </c>
@@ -4524,7 +4533,7 @@
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
     </row>
-    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="8" t="s">
         <v>61</v>
       </c>
@@ -4556,7 +4565,7 @@
       <c r="W55" s="2"/>
       <c r="X55" s="2"/>
     </row>
-    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="8" t="s">
         <v>61</v>
       </c>
@@ -4588,7 +4597,7 @@
       <c r="W56" s="2"/>
       <c r="X56" s="2"/>
     </row>
-    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="8" t="s">
         <v>61</v>
       </c>
@@ -4620,7 +4629,7 @@
       <c r="W57" s="2"/>
       <c r="X57" s="2"/>
     </row>
-    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="8" t="s">
         <v>61</v>
       </c>
@@ -4652,7 +4661,7 @@
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
     </row>
-    <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="9" t="s">
         <v>61</v>
       </c>
@@ -4684,7 +4693,7 @@
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
     </row>
-    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="9" t="s">
         <v>61</v>
       </c>
@@ -4716,7 +4725,7 @@
       <c r="W60" s="2"/>
       <c r="X60" s="2"/>
     </row>
-    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="9" t="s">
         <v>61</v>
       </c>
@@ -4750,7 +4759,7 @@
       <c r="W61" s="2"/>
       <c r="X61" s="2"/>
     </row>
-    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="16"/>
       <c r="B62" s="17"/>
       <c r="C62" s="7"/>
@@ -4776,7 +4785,7 @@
       <c r="W62" s="2"/>
       <c r="X62" s="2"/>
     </row>
-    <row r="63" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="16"/>
       <c r="B63" s="17"/>
       <c r="C63" s="7"/>
@@ -4802,7 +4811,7 @@
       <c r="W63" s="2"/>
       <c r="X63" s="2"/>
     </row>
-    <row r="64" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="8" t="s">
         <v>105</v>
       </c>
@@ -4834,7 +4843,7 @@
       <c r="W64" s="2"/>
       <c r="X64" s="2"/>
     </row>
-    <row r="65" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="8" t="s">
         <v>105</v>
       </c>
@@ -4866,7 +4875,7 @@
       <c r="W65" s="2"/>
       <c r="X65" s="2"/>
     </row>
-    <row r="66" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="8" t="s">
         <v>105</v>
       </c>
@@ -4898,7 +4907,7 @@
       <c r="W66" s="2"/>
       <c r="X66" s="2"/>
     </row>
-    <row r="67" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="8" t="s">
         <v>105</v>
       </c>
@@ -4930,7 +4939,7 @@
       <c r="W67" s="2"/>
       <c r="X67" s="2"/>
     </row>
-    <row r="68" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="8" t="s">
         <v>105</v>
       </c>
@@ -4962,7 +4971,7 @@
       <c r="W68" s="2"/>
       <c r="X68" s="2"/>
     </row>
-    <row r="69" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="8" t="s">
         <v>105</v>
       </c>
@@ -4996,7 +5005,7 @@
       <c r="W69" s="2"/>
       <c r="X69" s="2"/>
     </row>
-    <row r="70" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="8" t="s">
         <v>105</v>
       </c>
@@ -5028,7 +5037,7 @@
       <c r="W70" s="2"/>
       <c r="X70" s="2"/>
     </row>
-    <row r="71" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="8" t="s">
         <v>105</v>
       </c>
@@ -5060,7 +5069,7 @@
       <c r="W71" s="2"/>
       <c r="X71" s="2"/>
     </row>
-    <row r="72" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="8" t="s">
         <v>105</v>
       </c>
@@ -5092,7 +5101,7 @@
       <c r="W72" s="2"/>
       <c r="X72" s="2"/>
     </row>
-    <row r="73" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="9" t="s">
         <v>105</v>
       </c>
@@ -5124,7 +5133,7 @@
       <c r="W73" s="2"/>
       <c r="X73" s="2"/>
     </row>
-    <row r="74" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="18"/>
       <c r="B74" s="17"/>
       <c r="C74" s="7"/>
@@ -5150,7 +5159,7 @@
       <c r="W74" s="2"/>
       <c r="X74" s="2"/>
     </row>
-    <row r="75" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="18"/>
       <c r="B75" s="17"/>
       <c r="C75" s="7"/>
@@ -5176,7 +5185,7 @@
       <c r="W75" s="2"/>
       <c r="X75" s="2"/>
     </row>
-    <row r="76" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="19" t="s">
         <v>126</v>
       </c>
@@ -5208,7 +5217,7 @@
       <c r="W76" s="2"/>
       <c r="X76" s="2"/>
     </row>
-    <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="19" t="s">
         <v>126</v>
       </c>
@@ -5240,7 +5249,7 @@
       <c r="W77" s="2"/>
       <c r="X77" s="2"/>
     </row>
-    <row r="78" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="19" t="s">
         <v>126</v>
       </c>
@@ -5272,7 +5281,7 @@
       <c r="W78" s="2"/>
       <c r="X78" s="2"/>
     </row>
-    <row r="79" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="19" t="s">
         <v>126</v>
       </c>
@@ -5304,7 +5313,7 @@
       <c r="W79" s="2"/>
       <c r="X79" s="2"/>
     </row>
-    <row r="80" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="19" t="s">
         <v>126</v>
       </c>
@@ -7548,136 +7557,136 @@
       <c r="X151" s="2"/>
     </row>
     <row r="152" spans="1:26" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A152" s="52" t="s">
+      <c r="A152" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="B152" s="53" t="s">
+      <c r="B152" s="49" t="s">
         <v>254</v>
       </c>
-      <c r="C152" s="54" t="s">
+      <c r="C152" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="D152" s="55"/>
-      <c r="E152" s="55"/>
-      <c r="F152" s="55"/>
-      <c r="G152" s="55"/>
-      <c r="H152" s="55"/>
-      <c r="I152" s="55"/>
-      <c r="J152" s="55"/>
-      <c r="K152" s="55"/>
-      <c r="L152" s="55"/>
-      <c r="M152" s="55"/>
-      <c r="N152" s="55"/>
-      <c r="O152" s="55"/>
-      <c r="P152" s="55"/>
-      <c r="Q152" s="55"/>
-      <c r="R152" s="55"/>
-      <c r="S152" s="55"/>
-      <c r="T152" s="55"/>
-      <c r="U152" s="55"/>
-      <c r="V152" s="55"/>
-      <c r="W152" s="55"/>
-      <c r="X152" s="55"/>
-      <c r="Y152" s="56"/>
-      <c r="Z152" s="56"/>
+      <c r="D152" s="51"/>
+      <c r="E152" s="51"/>
+      <c r="F152" s="51"/>
+      <c r="G152" s="51"/>
+      <c r="H152" s="51"/>
+      <c r="I152" s="51"/>
+      <c r="J152" s="51"/>
+      <c r="K152" s="51"/>
+      <c r="L152" s="51"/>
+      <c r="M152" s="51"/>
+      <c r="N152" s="51"/>
+      <c r="O152" s="51"/>
+      <c r="P152" s="51"/>
+      <c r="Q152" s="51"/>
+      <c r="R152" s="51"/>
+      <c r="S152" s="51"/>
+      <c r="T152" s="51"/>
+      <c r="U152" s="51"/>
+      <c r="V152" s="51"/>
+      <c r="W152" s="51"/>
+      <c r="X152" s="51"/>
+      <c r="Y152" s="52"/>
+      <c r="Z152" s="52"/>
     </row>
     <row r="153" spans="1:26" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A153" s="57" t="s">
+      <c r="A153" s="53" t="s">
         <v>253</v>
       </c>
-      <c r="B153" s="58" t="s">
+      <c r="B153" s="54" t="s">
         <v>256</v>
       </c>
-      <c r="C153" s="59" t="s">
+      <c r="C153" s="55" t="s">
         <v>257</v>
       </c>
-      <c r="D153" s="60"/>
-      <c r="E153" s="61"/>
-      <c r="F153" s="61"/>
-      <c r="G153" s="61"/>
-      <c r="H153" s="61"/>
-      <c r="I153" s="61"/>
-      <c r="J153" s="61"/>
-      <c r="K153" s="61"/>
-      <c r="L153" s="61"/>
-      <c r="M153" s="61"/>
-      <c r="N153" s="61"/>
-      <c r="O153" s="61"/>
-      <c r="P153" s="61"/>
-      <c r="Q153" s="61"/>
-      <c r="R153" s="61"/>
-      <c r="S153" s="61"/>
-      <c r="T153" s="61"/>
-      <c r="U153" s="61"/>
-      <c r="V153" s="61"/>
-      <c r="W153" s="61"/>
-      <c r="X153" s="61"/>
-      <c r="Y153" s="62"/>
-      <c r="Z153" s="62"/>
-    </row>
-    <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A154" s="5" t="s">
+      <c r="D153" s="56"/>
+      <c r="E153" s="57"/>
+      <c r="F153" s="57"/>
+      <c r="G153" s="57"/>
+      <c r="H153" s="57"/>
+      <c r="I153" s="57"/>
+      <c r="J153" s="57"/>
+      <c r="K153" s="57"/>
+      <c r="L153" s="57"/>
+      <c r="M153" s="57"/>
+      <c r="N153" s="57"/>
+      <c r="O153" s="57"/>
+      <c r="P153" s="57"/>
+      <c r="Q153" s="57"/>
+      <c r="R153" s="57"/>
+      <c r="S153" s="57"/>
+      <c r="T153" s="57"/>
+      <c r="U153" s="57"/>
+      <c r="V153" s="57"/>
+      <c r="W153" s="57"/>
+      <c r="X153" s="57"/>
+      <c r="Y153" s="58"/>
+      <c r="Z153" s="58"/>
+    </row>
+    <row r="154" spans="1:26" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A154" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B154" s="44" t="s">
         <v>258</v>
       </c>
-      <c r="C154" s="13" t="s">
+      <c r="C154" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="D154" s="29"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
-      <c r="J154" s="2"/>
-      <c r="K154" s="2"/>
-      <c r="L154" s="2"/>
-      <c r="M154" s="2"/>
-      <c r="N154" s="2"/>
-      <c r="O154" s="2"/>
-      <c r="P154" s="2"/>
-      <c r="Q154" s="2"/>
-      <c r="R154" s="2"/>
-      <c r="S154" s="2"/>
-      <c r="T154" s="2"/>
-      <c r="U154" s="2"/>
-      <c r="V154" s="2"/>
-      <c r="W154" s="2"/>
-      <c r="X154" s="2"/>
-    </row>
-    <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A155" s="5" t="s">
+      <c r="D154" s="63"/>
+      <c r="E154" s="46"/>
+      <c r="F154" s="46"/>
+      <c r="G154" s="46"/>
+      <c r="H154" s="46"/>
+      <c r="I154" s="46"/>
+      <c r="J154" s="46"/>
+      <c r="K154" s="46"/>
+      <c r="L154" s="46"/>
+      <c r="M154" s="46"/>
+      <c r="N154" s="46"/>
+      <c r="O154" s="46"/>
+      <c r="P154" s="46"/>
+      <c r="Q154" s="46"/>
+      <c r="R154" s="46"/>
+      <c r="S154" s="46"/>
+      <c r="T154" s="46"/>
+      <c r="U154" s="46"/>
+      <c r="V154" s="46"/>
+      <c r="W154" s="46"/>
+      <c r="X154" s="46"/>
+    </row>
+    <row r="155" spans="1:26" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="B155" s="14" t="s">
+      <c r="B155" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="C155" s="13" t="s">
+      <c r="C155" s="45" t="s">
         <v>261</v>
       </c>
-      <c r="D155" s="29"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
-      <c r="G155" s="2"/>
-      <c r="H155" s="2"/>
-      <c r="I155" s="2"/>
-      <c r="J155" s="2"/>
-      <c r="K155" s="2"/>
-      <c r="L155" s="2"/>
-      <c r="M155" s="2"/>
-      <c r="N155" s="2"/>
-      <c r="O155" s="2"/>
-      <c r="P155" s="2"/>
-      <c r="Q155" s="2"/>
-      <c r="R155" s="2"/>
-      <c r="S155" s="2"/>
-      <c r="T155" s="2"/>
-      <c r="U155" s="2"/>
-      <c r="V155" s="2"/>
-      <c r="W155" s="2"/>
-      <c r="X155" s="2"/>
+      <c r="D155" s="63"/>
+      <c r="E155" s="46"/>
+      <c r="F155" s="46"/>
+      <c r="G155" s="46"/>
+      <c r="H155" s="46"/>
+      <c r="I155" s="46"/>
+      <c r="J155" s="46"/>
+      <c r="K155" s="46"/>
+      <c r="L155" s="46"/>
+      <c r="M155" s="46"/>
+      <c r="N155" s="46"/>
+      <c r="O155" s="46"/>
+      <c r="P155" s="46"/>
+      <c r="Q155" s="46"/>
+      <c r="R155" s="46"/>
+      <c r="S155" s="46"/>
+      <c r="T155" s="46"/>
+      <c r="U155" s="46"/>
+      <c r="V155" s="46"/>
+      <c r="W155" s="46"/>
+      <c r="X155" s="46"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="5" t="s">
@@ -7711,37 +7720,37 @@
       <c r="W156" s="2"/>
       <c r="X156" s="2"/>
     </row>
-    <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A157" s="5" t="s">
+    <row r="157" spans="1:26" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A157" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="B157" s="14" t="s">
+      <c r="B157" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="C157" s="13" t="s">
+      <c r="C157" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="D157" s="29"/>
-      <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
-      <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-      <c r="I157" s="2"/>
-      <c r="J157" s="2"/>
-      <c r="K157" s="2"/>
-      <c r="L157" s="2"/>
-      <c r="M157" s="2"/>
-      <c r="N157" s="2"/>
-      <c r="O157" s="2"/>
-      <c r="P157" s="2"/>
-      <c r="Q157" s="2"/>
-      <c r="R157" s="2"/>
-      <c r="S157" s="2"/>
-      <c r="T157" s="2"/>
-      <c r="U157" s="2"/>
-      <c r="V157" s="2"/>
-      <c r="W157" s="2"/>
-      <c r="X157" s="2"/>
+      <c r="D157" s="63"/>
+      <c r="E157" s="46"/>
+      <c r="F157" s="46"/>
+      <c r="G157" s="46"/>
+      <c r="H157" s="46"/>
+      <c r="I157" s="46"/>
+      <c r="J157" s="46"/>
+      <c r="K157" s="46"/>
+      <c r="L157" s="46"/>
+      <c r="M157" s="46"/>
+      <c r="N157" s="46"/>
+      <c r="O157" s="46"/>
+      <c r="P157" s="46"/>
+      <c r="Q157" s="46"/>
+      <c r="R157" s="46"/>
+      <c r="S157" s="46"/>
+      <c r="T157" s="46"/>
+      <c r="U157" s="46"/>
+      <c r="V157" s="46"/>
+      <c r="W157" s="46"/>
+      <c r="X157" s="46"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="8" t="s">
@@ -21368,39 +21377,39 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DB562CAF-E1A0-40F3-9192-5E17BE155BA5}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A6CE0597-98E5-4A5B-AB5F-6EEE71119C0A}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{0F3B6852-6A7A-46DF-9AF2-9E75C4D61840}"/>
+      <autoFilter ref="A11:C37" xr:uid="{19B65649-6521-4AFA-A1B3-E330D03FF921}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1247552191"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="418346103"/>
+        </ext>
+      </extLst>
+    </customSheetView>
+    <customSheetView guid="{FB58D069-98FB-40A6-98B6-6F873CC8E3CF}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{AAA5C973-A249-475F-A022-812DFF1B2338}"/>
+      <extLst>
+        <ext uri="GoogleSheetsCustomDataVersion1">
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2099002125"/>
         </ext>
       </extLst>
     </customSheetView>
     <customSheetView guid="{C68DABDE-8AC1-49C3-98CF-691EE57ABE88}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{9F76F1C4-F905-435F-B686-174F1960369F}"/>
+      <autoFilter ref="A293:C332" xr:uid="{3CEDEE09-C182-40CE-847E-A3C670121D35}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
           <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1542537633"/>
         </ext>
       </extLst>
     </customSheetView>
-    <customSheetView guid="{FB58D069-98FB-40A6-98B6-6F873CC8E3CF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DB562CAF-E1A0-40F3-9192-5E17BE155BA5}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{41107013-996E-4B6D-806F-FFCDA3D6B302}"/>
+      <autoFilter ref="A11:D37" xr:uid="{47911D17-7E56-4593-ABFD-11BAC1B31A9B}"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="2099002125"/>
-        </ext>
-      </extLst>
-    </customSheetView>
-    <customSheetView guid="{A6CE0597-98E5-4A5B-AB5F-6EEE71119C0A}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{3D1507BF-AF02-498D-B191-89DE8EC6B919}"/>
-      <extLst>
-        <ext uri="GoogleSheetsCustomDataVersion1">
-          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="418346103"/>
+          <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" filterViewId="1247552191"/>
         </ext>
       </extLst>
     </customSheetView>
@@ -21813,35 +21822,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="60"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -21850,7 +21859,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -21859,7 +21868,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
@@ -21868,7 +21877,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -21885,7 +21894,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
         <v>61</v>
       </c>
@@ -21956,7 +21965,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
         <v>169</v>
       </c>
@@ -21964,7 +21973,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="9" t="s">
         <v>169</v>
       </c>
@@ -21972,15 +21981,15 @@
         <v>667</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="42"/>
       <c r="B26" s="14"/>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="42"/>
       <c r="B27" s="14"/>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="8" t="s">
         <v>203</v>
       </c>
@@ -21988,7 +21997,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
         <v>203</v>
       </c>
@@ -21996,7 +22005,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="9" t="s">
         <v>203</v>
       </c>
@@ -22004,7 +22013,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="9" t="s">
         <v>203</v>
       </c>
@@ -22012,7 +22021,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="9" t="s">
         <v>203</v>
       </c>
@@ -22020,15 +22029,15 @@
         <v>672</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="42"/>
       <c r="B33" s="14"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="42"/>
       <c r="B34" s="14"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="8" t="s">
         <v>253</v>
       </c>
@@ -22036,7 +22045,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="9" t="s">
         <v>253</v>
       </c>
@@ -22044,7 +22053,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="9" t="s">
         <v>253</v>
       </c>

</xml_diff>